<commit_message>
Completed Week 7&8 Exercise
</commit_message>
<xml_diff>
--- a/Weekly Exercises/Weeks 7 & 8 Data/CANDYDATA.xlsx
+++ b/Weekly Exercises/Weeks 7 & 8 Data/CANDYDATA.xlsx
@@ -1,16 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bellevueuniversity-my.sharepoint.com/personal/plozano_my365_bellevue_edu/Documents/DSC540-T302 Data Preparation/The-Data-Wrangling-Workshop/Weekly Exercises/Weeks 7 &amp; 8 Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_6E4D8D962E7FBFC02371D822FCEC84732426185C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E28E686-897A-4132-8CEC-E071DDB158A1}"/>
   <bookViews>
-    <workbookView xWindow="34740" yWindow="1160" windowWidth="48780" windowHeight="28180" tabRatio="500"/>
+    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130405" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -309,8 +326,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -353,29 +370,47 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0521364446232542"/>
-          <c:y val="0.0237262350310998"/>
-          <c:w val="0.854439335594"/>
-          <c:h val="0.963954373702752"/>
+          <c:x val="5.2136444623254202E-2"/>
+          <c:y val="2.3726235031099802E-2"/>
+          <c:w val="0.85443933559399998"/>
+          <c:h val="0.96395437370275205"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -676,266 +711,272 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="86"/>
                 <c:pt idx="0">
-                  <c:v>634.0</c:v>
+                  <c:v>634</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>323.0</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>770.0</c:v>
+                  <c:v>770</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>81.0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>627.0</c:v>
+                  <c:v>627</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>534.0</c:v>
+                  <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>135.0</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>470.0</c:v>
+                  <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>500.0</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>739.0</c:v>
+                  <c:v>739</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>206.0</c:v>
+                  <c:v>206</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>406.0</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>511.0</c:v>
+                  <c:v>511</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>46.0</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>230.0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>635.0</c:v>
+                  <c:v>635</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>74.0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>629.0</c:v>
+                  <c:v>629</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>59.0</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>983.0</c:v>
+                  <c:v>983</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>279.0</c:v>
+                  <c:v>279</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39.0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>773.0</c:v>
+                  <c:v>773</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>166.0</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>168.0</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>565.0</c:v>
+                  <c:v>565</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>514.0</c:v>
+                  <c:v>514</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>335.0</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>58.0</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>171.0</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>154.0</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>186.0</c:v>
+                  <c:v>186</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>648.0</c:v>
+                  <c:v>648</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>541.0</c:v>
+                  <c:v>541</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>37.0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>163.0</c:v>
+                  <c:v>163</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>166.0</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>551.0</c:v>
+                  <c:v>551</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>256.0</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>287.0</c:v>
+                  <c:v>287</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>352.0</c:v>
+                  <c:v>352</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>293.0</c:v>
+                  <c:v>293</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>894.0</c:v>
+                  <c:v>894</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>145.0</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>51.0</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>550.0</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>466.0</c:v>
+                  <c:v>466</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>160.0</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>510.0</c:v>
+                  <c:v>510</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>314.0</c:v>
+                  <c:v>314</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>568.0</c:v>
+                  <c:v>568</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>74.0</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>400.0</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>21.0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>204.0</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>171.0</c:v>
+                  <c:v>171</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>219.0</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>188.0</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>272.0</c:v>
+                  <c:v>272</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>43.0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>586.0</c:v>
+                  <c:v>586</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>126.0</c:v>
+                  <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>132.0</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>642.0</c:v>
+                  <c:v>642</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>493.0</c:v>
+                  <c:v>493</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>29.0</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>457.0</c:v>
+                  <c:v>457</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>579.0</c:v>
+                  <c:v>579</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>115.0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>14.0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>115.0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>31.0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>34.0</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>828.0</c:v>
+                  <c:v>828</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>570.0</c:v>
+                  <c:v>570</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-35E5-45EB-A63D-5CEEC6C56AAD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1227,266 +1268,272 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="86"/>
                 <c:pt idx="0">
-                  <c:v>556.0</c:v>
+                  <c:v>556</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-398.0</c:v>
+                  <c:v>-398</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-458.0</c:v>
+                  <c:v>-458</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113.0</c:v>
+                  <c:v>113</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>744.0</c:v>
+                  <c:v>744</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-166.0</c:v>
+                  <c:v>-166</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>583.0</c:v>
+                  <c:v>583</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>494.0</c:v>
+                  <c:v>494</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-410.0</c:v>
+                  <c:v>-410</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-71.0</c:v>
+                  <c:v>-71</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>304.0</c:v>
+                  <c:v>304</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>431.0</c:v>
+                  <c:v>431</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-224.0</c:v>
+                  <c:v>-224</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>712.0</c:v>
+                  <c:v>712</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>115.0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>219.0</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>419.0</c:v>
+                  <c:v>419</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-111.0</c:v>
+                  <c:v>-111</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>82.0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>585.0</c:v>
+                  <c:v>585</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-206.0</c:v>
+                  <c:v>-206</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>588.0</c:v>
+                  <c:v>588</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-15.0</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>936.0</c:v>
+                  <c:v>936</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>115.0</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-328.0</c:v>
+                  <c:v>-328</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>698.0</c:v>
+                  <c:v>698</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>127.0</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-32.0</c:v>
+                  <c:v>-32</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>526.0</c:v>
+                  <c:v>526</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>399.0</c:v>
+                  <c:v>399</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>219.0</c:v>
+                  <c:v>219</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-114.0</c:v>
+                  <c:v>-114</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>69.0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>56.0</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>52.0</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>615.0</c:v>
+                  <c:v>615</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>441.0</c:v>
+                  <c:v>441</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-31.0</c:v>
+                  <c:v>-31</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>33.0</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>519.0</c:v>
+                  <c:v>519</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>45.0</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-151.0</c:v>
+                  <c:v>-151</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>230.0</c:v>
+                  <c:v>230</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-255.0</c:v>
+                  <c:v>-255</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>82.0</c:v>
+                  <c:v>82</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>879.0</c:v>
+                  <c:v>879</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>38.0</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-446.0</c:v>
+                  <c:v>-446</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>490.0</c:v>
+                  <c:v>490</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>300.0</c:v>
+                  <c:v>300</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-366.0</c:v>
+                  <c:v>-366</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-108.0</c:v>
+                  <c:v>-108</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>425.0</c:v>
+                  <c:v>425</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>249.0</c:v>
+                  <c:v>249</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>507.0</c:v>
+                  <c:v>507</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-251.0</c:v>
+                  <c:v>-251</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-169.0</c:v>
+                  <c:v>-169</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>253.0</c:v>
+                  <c:v>253</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-450.0</c:v>
+                  <c:v>-450</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-88.0</c:v>
+                  <c:v>-88</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>55.0</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>91.0</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-377.0</c:v>
+                  <c:v>-377</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-19.0</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>47.0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-543.0</c:v>
+                  <c:v>-543</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>504.0</c:v>
+                  <c:v>504</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-481.0</c:v>
+                  <c:v>-481</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-153.0</c:v>
+                  <c:v>-153</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>599.0</c:v>
+                  <c:v>599</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>460.0</c:v>
+                  <c:v>460</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-592.0</c:v>
+                  <c:v>-592</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>130.0</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>435.0</c:v>
+                  <c:v>435</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-162.0</c:v>
+                  <c:v>-162</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-565.0</c:v>
+                  <c:v>-565</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-166.0</c:v>
+                  <c:v>-166</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-538.0</c:v>
+                  <c:v>-538</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>81.0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-68.0</c:v>
+                  <c:v>-68</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-218.0</c:v>
+                  <c:v>-218</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>815.0</c:v>
+                  <c:v>815</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-543.0</c:v>
+                  <c:v>-543</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>536.0</c:v>
+                  <c:v>536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-35E5-45EB-A63D-5CEEC6C56AAD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1787,269 +1834,282 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="86"/>
                 <c:pt idx="0">
-                  <c:v>-78.0</c:v>
+                  <c:v>-78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-419.0</c:v>
+                  <c:v>-419</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-473.0</c:v>
+                  <c:v>-473</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-210.0</c:v>
+                  <c:v>-210</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-26.0</c:v>
+                  <c:v>-26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-247.0</c:v>
+                  <c:v>-247</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-44.0</c:v>
+                  <c:v>-44</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-40.0</c:v>
+                  <c:v>-40</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-545.0</c:v>
+                  <c:v>-545</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-92.0</c:v>
+                  <c:v>-92</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-166.0</c:v>
+                  <c:v>-166</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-69.0</c:v>
+                  <c:v>-69</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-253.0</c:v>
+                  <c:v>-253</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-27.0</c:v>
+                  <c:v>-27</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-91.0</c:v>
+                  <c:v>-91</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-187.0</c:v>
+                  <c:v>-187</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-92.0</c:v>
+                  <c:v>-92</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-157.0</c:v>
+                  <c:v>-157</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-148.0</c:v>
+                  <c:v>-148</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-50.0</c:v>
+                  <c:v>-50</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-280.0</c:v>
+                  <c:v>-280</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-41.0</c:v>
+                  <c:v>-41</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-74.0</c:v>
+                  <c:v>-74</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-47.0</c:v>
+                  <c:v>-47</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-164.0</c:v>
+                  <c:v>-164</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-367.0</c:v>
+                  <c:v>-367</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-75.0</c:v>
+                  <c:v>-75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-39.0</c:v>
+                  <c:v>-39</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-200.0</c:v>
+                  <c:v>-200</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-39.0</c:v>
+                  <c:v>-39</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-115.0</c:v>
+                  <c:v>-115</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-116.0</c:v>
+                  <c:v>-116</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-172.0</c:v>
+                  <c:v>-172</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-102.0</c:v>
+                  <c:v>-102</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-98.0</c:v>
+                  <c:v>-98</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-134.0</c:v>
+                  <c:v>-134</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-33.0</c:v>
+                  <c:v>-33</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-100.0</c:v>
+                  <c:v>-100</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-68.0</c:v>
+                  <c:v>-68</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-163.0</c:v>
+                  <c:v>-163</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-133.0</c:v>
+                  <c:v>-133</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-32.0</c:v>
+                  <c:v>-32</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-211.0</c:v>
+                  <c:v>-211</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-438.0</c:v>
+                  <c:v>-438</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-122.0</c:v>
+                  <c:v>-122</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-285.0</c:v>
+                  <c:v>-285</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-211.0</c:v>
+                  <c:v>-211</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-15.0</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-107.0</c:v>
+                  <c:v>-107</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-497.0</c:v>
+                  <c:v>-497</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-60.0</c:v>
+                  <c:v>-60</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-166.0</c:v>
+                  <c:v>-166</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-421.0</c:v>
+                  <c:v>-421</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-268.0</c:v>
+                  <c:v>-268</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-85.0</c:v>
+                  <c:v>-85</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>-65.0</c:v>
+                  <c:v>-65</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-61.0</c:v>
+                  <c:v>-61</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>-325.0</c:v>
+                  <c:v>-325</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-299.0</c:v>
+                  <c:v>-299</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>-147.0</c:v>
+                  <c:v>-147</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-471.0</c:v>
+                  <c:v>-471</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>-292.0</c:v>
+                  <c:v>-292</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>-116.0</c:v>
+                  <c:v>-116</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-128.0</c:v>
+                  <c:v>-128</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>-415.0</c:v>
+                  <c:v>-415</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-207.0</c:v>
+                  <c:v>-207</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-225.0</c:v>
+                  <c:v>-225</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-586.0</c:v>
+                  <c:v>-586</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-82.0</c:v>
+                  <c:v>-82</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-607.0</c:v>
+                  <c:v>-607</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>-285.0</c:v>
+                  <c:v>-285</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>-43.0</c:v>
+                  <c:v>-43</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>-33.0</c:v>
+                  <c:v>-33</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>-621.0</c:v>
+                  <c:v>-621</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>-327.0</c:v>
+                  <c:v>-327</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>-144.0</c:v>
+                  <c:v>-144</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>-277.0</c:v>
+                  <c:v>-277</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>-579.0</c:v>
+                  <c:v>-579</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>-281.0</c:v>
+                  <c:v>-281</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>-585.0</c:v>
+                  <c:v>-585</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>-219.0</c:v>
+                  <c:v>-219</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>-99.0</c:v>
+                  <c:v>-99</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>-252.0</c:v>
+                  <c:v>-252</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>-13.0</c:v>
+                  <c:v>-13</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>-663.0</c:v>
+                  <c:v>-663</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>-34.0</c:v>
+                  <c:v>-34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-35E5-45EB-A63D-5CEEC6C56AAD}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
-        <c:dLbls/>
-        <c:marker val="1"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
         <c:axId val="598350696"/>
         <c:axId val="588600840"/>
       </c:lineChart>
@@ -2058,7 +2118,11 @@
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -2075,12 +2139,14 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="588600840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
@@ -2114,6 +2180,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:ln>
@@ -2134,7 +2201,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2144,20 +2211,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>901700</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>132080</xdr:colOff>
       <xdr:row>80</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>86360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2173,6 +2246,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2494,23 +2571,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <sheetPr published="0" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr published="0"/>
   <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="10.7265625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="34.26953125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.54296875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2530,7 +2607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2541,19 +2618,19 @@
         <v>78</v>
       </c>
       <c r="D2" s="1">
-        <f>B2-C2</f>
+        <f t="shared" ref="D2:D33" si="0">B2-C2</f>
         <v>556</v>
       </c>
       <c r="E2" s="1">
-        <f>(B2+C2)/(434.38)</f>
+        <f t="shared" ref="E2:E33" si="1">(B2+C2)/(434.38)</f>
         <v>1.6391178231041945</v>
       </c>
       <c r="F2" s="1">
-        <f>-(C2)</f>
+        <f t="shared" ref="F2:F33" si="2">-(C2)</f>
         <v>-78</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2564,19 +2641,19 @@
         <v>419</v>
       </c>
       <c r="D3" s="1">
-        <f>B3-C3</f>
+        <f t="shared" si="0"/>
         <v>-398</v>
       </c>
       <c r="E3" s="1">
-        <f>(B3+C3)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.0129379805700078</v>
       </c>
       <c r="F3" s="1">
-        <f>-(C3)</f>
+        <f t="shared" si="2"/>
         <v>-419</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -2587,19 +2664,19 @@
         <v>473</v>
       </c>
       <c r="D4" s="1">
-        <f>B4-C4</f>
+        <f t="shared" si="0"/>
         <v>-458</v>
       </c>
       <c r="E4" s="1">
-        <f>(B4+C4)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.1234403057230995</v>
       </c>
       <c r="F4" s="1">
-        <f>-(C4)</f>
+        <f t="shared" si="2"/>
         <v>-473</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2610,19 +2687,19 @@
         <v>210</v>
       </c>
       <c r="D5" s="1">
-        <f>B5-C5</f>
+        <f t="shared" si="0"/>
         <v>113</v>
       </c>
       <c r="E5" s="1">
-        <f>(B5+C5)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.2270362355541231</v>
       </c>
       <c r="F5" s="1">
-        <f>-(C5)</f>
+        <f t="shared" si="2"/>
         <v>-210</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -2633,19 +2710,19 @@
         <v>26</v>
       </c>
       <c r="D6" s="1">
-        <f>B6-C6</f>
+        <f t="shared" si="0"/>
         <v>744</v>
       </c>
       <c r="E6" s="1">
-        <f>(B6+C6)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.832496892122105</v>
       </c>
       <c r="F6" s="1">
-        <f>-(C6)</f>
+        <f t="shared" si="2"/>
         <v>-26</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -2656,19 +2733,19 @@
         <v>247</v>
       </c>
       <c r="D7" s="1">
-        <f>B7-C7</f>
+        <f t="shared" si="0"/>
         <v>-166</v>
       </c>
       <c r="E7" s="1">
-        <f>(B7+C7)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.75509922187946044</v>
       </c>
       <c r="F7" s="1">
-        <f>-(C7)</f>
+        <f t="shared" si="2"/>
         <v>-247</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2679,19 +2756,19 @@
         <v>44</v>
       </c>
       <c r="D8" s="1">
-        <f>B8-C8</f>
+        <f t="shared" si="0"/>
         <v>583</v>
       </c>
       <c r="E8" s="1">
-        <f>(B8+C8)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.544730420369262</v>
       </c>
       <c r="F8" s="1">
-        <f>-(C8)</f>
+        <f t="shared" si="2"/>
         <v>-44</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>91</v>
       </c>
@@ -2702,19 +2779,19 @@
         <v>40</v>
       </c>
       <c r="D9" s="1">
-        <f>B9-C9</f>
+        <f t="shared" si="0"/>
         <v>494</v>
       </c>
       <c r="E9" s="1">
-        <f>(B9+C9)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.3214236382890556</v>
       </c>
       <c r="F9" s="1">
-        <f>-(C9)</f>
+        <f t="shared" si="2"/>
         <v>-40</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
@@ -2725,19 +2802,19 @@
         <v>545</v>
       </c>
       <c r="D10" s="1">
-        <f>B10-C10</f>
+        <f t="shared" si="0"/>
         <v>-410</v>
       </c>
       <c r="E10" s="1">
-        <f>(B10+C10)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.5654496063354666</v>
       </c>
       <c r="F10" s="1">
-        <f>-(C10)</f>
+        <f t="shared" si="2"/>
         <v>-545</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>89</v>
       </c>
@@ -2748,19 +2825,19 @@
         <v>92</v>
       </c>
       <c r="D11" s="1">
-        <f>B11-C11</f>
+        <f t="shared" si="0"/>
         <v>-71</v>
       </c>
       <c r="E11" s="1">
-        <f>(B11+C11)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.26014089046457017</v>
       </c>
       <c r="F11" s="1">
-        <f>-(C11)</f>
+        <f t="shared" si="2"/>
         <v>-92</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>88</v>
       </c>
@@ -2771,19 +2848,19 @@
         <v>166</v>
       </c>
       <c r="D12" s="1">
-        <f>B12-C12</f>
+        <f t="shared" si="0"/>
         <v>304</v>
       </c>
       <c r="E12" s="1">
-        <f>(B12+C12)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.4641558082784658</v>
       </c>
       <c r="F12" s="1">
-        <f>-(C12)</f>
+        <f t="shared" si="2"/>
         <v>-166</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>87</v>
       </c>
@@ -2794,19 +2871,19 @@
         <v>69</v>
       </c>
       <c r="D13" s="1">
-        <f>B13-C13</f>
+        <f t="shared" si="0"/>
         <v>431</v>
       </c>
       <c r="E13" s="1">
-        <f>(B13+C13)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.3099129794189419</v>
       </c>
       <c r="F13" s="1">
-        <f>-(C13)</f>
+        <f t="shared" si="2"/>
         <v>-69</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>86</v>
       </c>
@@ -2817,19 +2894,19 @@
         <v>253</v>
       </c>
       <c r="D14" s="1">
-        <f>B14-C14</f>
+        <f t="shared" si="0"/>
         <v>-224</v>
       </c>
       <c r="E14" s="1">
-        <f>(B14+C14)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.6492011602744141</v>
       </c>
       <c r="F14" s="1">
-        <f>-(C14)</f>
+        <f t="shared" si="2"/>
         <v>-253</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>85</v>
       </c>
@@ -2840,19 +2917,19 @@
         <v>27</v>
       </c>
       <c r="D15" s="1">
-        <f>B15-C15</f>
+        <f t="shared" si="0"/>
         <v>712</v>
       </c>
       <c r="E15" s="1">
-        <f>(B15+C15)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.7634329389014227</v>
       </c>
       <c r="F15" s="1">
-        <f>-(C15)</f>
+        <f t="shared" si="2"/>
         <v>-27</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>84</v>
       </c>
@@ -2863,19 +2940,19 @@
         <v>91</v>
       </c>
       <c r="D16" s="1">
-        <f>B16-C16</f>
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="E16" s="1">
-        <f>(B16+C16)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.68373313688475534</v>
       </c>
       <c r="F16" s="1">
-        <f>-(C16)</f>
+        <f t="shared" si="2"/>
         <v>-91</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>83</v>
       </c>
@@ -2886,19 +2963,19 @@
         <v>187</v>
       </c>
       <c r="D17" s="1">
-        <f>B17-C17</f>
+        <f t="shared" si="0"/>
         <v>219</v>
       </c>
       <c r="E17" s="1">
-        <f>(B17+C17)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.3651641419954879</v>
       </c>
       <c r="F17" s="1">
-        <f>-(C17)</f>
+        <f t="shared" si="2"/>
         <v>-187</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>82</v>
       </c>
@@ -2909,19 +2986,19 @@
         <v>92</v>
       </c>
       <c r="D18" s="1">
-        <f>B18-C18</f>
+        <f t="shared" si="0"/>
         <v>419</v>
       </c>
       <c r="E18" s="1">
-        <f>(B18+C18)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.3881854597357153</v>
       </c>
       <c r="F18" s="1">
-        <f>-(C18)</f>
+        <f t="shared" si="2"/>
         <v>-92</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>81</v>
       </c>
@@ -2932,19 +3009,19 @@
         <v>157</v>
       </c>
       <c r="D19" s="1">
-        <f>B19-C19</f>
+        <f t="shared" si="0"/>
         <v>-111</v>
       </c>
       <c r="E19" s="1">
-        <f>(B19+C19)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.46733275012661724</v>
       </c>
       <c r="F19" s="1">
-        <f>-(C19)</f>
+        <f t="shared" si="2"/>
         <v>-157</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
@@ -2955,19 +3032,19 @@
         <v>148</v>
       </c>
       <c r="D20" s="1">
-        <f>B20-C20</f>
+        <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="E20" s="1">
-        <f>(B20+C20)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.87020581058059765</v>
       </c>
       <c r="F20" s="1">
-        <f>-(C20)</f>
+        <f t="shared" si="2"/>
         <v>-148</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -2978,19 +3055,19 @@
         <v>50</v>
       </c>
       <c r="D21" s="1">
-        <f>B21-C21</f>
+        <f t="shared" si="0"/>
         <v>585</v>
       </c>
       <c r="E21" s="1">
-        <f>(B21+C21)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.5769602652055803</v>
       </c>
       <c r="F21" s="1">
-        <f>-(C21)</f>
+        <f t="shared" si="2"/>
         <v>-50</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -3001,19 +3078,19 @@
         <v>280</v>
       </c>
       <c r="D22" s="1">
-        <f>B22-C22</f>
+        <f t="shared" si="0"/>
         <v>-206</v>
       </c>
       <c r="E22" s="1">
-        <f>(B22+C22)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.81495464800405171</v>
       </c>
       <c r="F22" s="1">
-        <f>-(C22)</f>
+        <f t="shared" si="2"/>
         <v>-280</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>77</v>
       </c>
@@ -3024,19 +3101,19 @@
         <v>41</v>
       </c>
       <c r="D23" s="1">
-        <f>B23-C23</f>
+        <f t="shared" si="0"/>
         <v>588</v>
       </c>
       <c r="E23" s="1">
-        <f>(B23+C23)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.5424282885952392</v>
       </c>
       <c r="F23" s="1">
-        <f>-(C23)</f>
+        <f t="shared" si="2"/>
         <v>-41</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>76</v>
       </c>
@@ -3047,19 +3124,19 @@
         <v>74</v>
       </c>
       <c r="D24" s="1">
-        <f>B24-C24</f>
+        <f t="shared" si="0"/>
         <v>-15</v>
       </c>
       <c r="E24" s="1">
-        <f>(B24+C24)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.30618352594502507</v>
       </c>
       <c r="F24" s="1">
-        <f>-(C24)</f>
+        <f t="shared" si="2"/>
         <v>-74</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
@@ -3070,19 +3147,19 @@
         <v>47</v>
       </c>
       <c r="D25" s="1">
-        <f>B25-C25</f>
+        <f t="shared" si="0"/>
         <v>936</v>
       </c>
       <c r="E25" s="1">
-        <f>(B25+C25)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>2.3711957272434274</v>
       </c>
       <c r="F25" s="1">
-        <f>-(C25)</f>
+        <f t="shared" si="2"/>
         <v>-47</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>74</v>
       </c>
@@ -3093,19 +3170,19 @@
         <v>164</v>
       </c>
       <c r="D26" s="1">
-        <f>B26-C26</f>
+        <f t="shared" si="0"/>
         <v>115</v>
       </c>
       <c r="E26" s="1">
-        <f>(B26+C26)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.0198443758920761</v>
       </c>
       <c r="F26" s="1">
-        <f>-(C26)</f>
+        <f t="shared" si="2"/>
         <v>-164</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>73</v>
       </c>
@@ -3116,19 +3193,19 @@
         <v>367</v>
       </c>
       <c r="D27" s="1">
-        <f>B27-C27</f>
+        <f t="shared" si="0"/>
         <v>-328</v>
       </c>
       <c r="E27" s="1">
-        <f>(B27+C27)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.93466550025323447</v>
       </c>
       <c r="F27" s="1">
-        <f>-(C27)</f>
+        <f t="shared" si="2"/>
         <v>-367</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -3139,19 +3216,19 @@
         <v>75</v>
       </c>
       <c r="D28" s="1">
-        <f>B28-C28</f>
+        <f t="shared" si="0"/>
         <v>698</v>
       </c>
       <c r="E28" s="1">
-        <f>(B28+C28)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.9522077443712877</v>
       </c>
       <c r="F28" s="1">
-        <f>-(C28)</f>
+        <f t="shared" si="2"/>
         <v>-75</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -3162,19 +3239,19 @@
         <v>39</v>
       </c>
       <c r="D29" s="1">
-        <f>B29-C29</f>
+        <f t="shared" si="0"/>
         <v>127</v>
       </c>
       <c r="E29" s="1">
-        <f>(B29+C29)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.47193701367466273</v>
       </c>
       <c r="F29" s="1">
-        <f>-(C29)</f>
+        <f t="shared" si="2"/>
         <v>-39</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
@@ -3185,19 +3262,19 @@
         <v>200</v>
       </c>
       <c r="D30" s="1">
-        <f>B30-C30</f>
+        <f t="shared" si="0"/>
         <v>-32</v>
       </c>
       <c r="E30" s="1">
-        <f>(B30+C30)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>0.84718449284037023</v>
       </c>
       <c r="F30" s="1">
-        <f>-(C30)</f>
+        <f t="shared" si="2"/>
         <v>-200</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>70</v>
       </c>
@@ -3208,19 +3285,19 @@
         <v>39</v>
       </c>
       <c r="D31" s="1">
-        <f>B31-C31</f>
+        <f t="shared" si="0"/>
         <v>526</v>
       </c>
       <c r="E31" s="1">
-        <f>(B31+C31)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.3904875915097381</v>
       </c>
       <c r="F31" s="1">
-        <f>-(C31)</f>
+        <f t="shared" si="2"/>
         <v>-39</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>69</v>
       </c>
@@ -3231,19 +3308,19 @@
         <v>115</v>
       </c>
       <c r="D32" s="1">
-        <f>B32-C32</f>
+        <f t="shared" si="0"/>
         <v>399</v>
       </c>
       <c r="E32" s="1">
-        <f>(B32+C32)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.4480408858603067</v>
       </c>
       <c r="F32" s="1">
-        <f>-(C32)</f>
+        <f t="shared" si="2"/>
         <v>-115</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>68</v>
       </c>
@@ -3254,19 +3331,19 @@
         <v>116</v>
       </c>
       <c r="D33" s="1">
-        <f>B33-C33</f>
+        <f t="shared" si="0"/>
         <v>219</v>
       </c>
       <c r="E33" s="1">
-        <f>(B33+C33)/(434.38)</f>
+        <f t="shared" si="1"/>
         <v>1.0382614300842581</v>
       </c>
       <c r="F33" s="1">
-        <f>-(C33)</f>
+        <f t="shared" si="2"/>
         <v>-116</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>67</v>
       </c>
@@ -3277,19 +3354,19 @@
         <v>172</v>
       </c>
       <c r="D34" s="1">
-        <f>B34-C34</f>
+        <f t="shared" ref="D34:D65" si="3">B34-C34</f>
         <v>-114</v>
       </c>
       <c r="E34" s="1">
-        <f>(B34+C34)/(434.38)</f>
+        <f t="shared" ref="E34:E65" si="4">(B34+C34)/(434.38)</f>
         <v>0.52949030802523134</v>
       </c>
       <c r="F34" s="1">
-        <f>-(C34)</f>
+        <f t="shared" ref="F34:F65" si="5">-(C34)</f>
         <v>-172</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>66</v>
       </c>
@@ -3300,19 +3377,19 @@
         <v>102</v>
       </c>
       <c r="D35" s="1">
-        <f>B35-C35</f>
+        <f t="shared" si="3"/>
         <v>69</v>
       </c>
       <c r="E35" s="1">
-        <f>(B35+C35)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.6284819743082094</v>
       </c>
       <c r="F35" s="1">
-        <f>-(C35)</f>
+        <f t="shared" si="5"/>
         <v>-102</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>65</v>
       </c>
@@ -3323,19 +3400,19 @@
         <v>98</v>
       </c>
       <c r="D36" s="1">
-        <f>B36-C36</f>
+        <f t="shared" si="3"/>
         <v>56</v>
       </c>
       <c r="E36" s="1">
-        <f>(B36+C36)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.58013720705373173</v>
       </c>
       <c r="F36" s="1">
-        <f>-(C36)</f>
+        <f t="shared" si="5"/>
         <v>-98</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>64</v>
       </c>
@@ -3346,19 +3423,19 @@
         <v>134</v>
       </c>
       <c r="D37" s="1">
-        <f>B37-C37</f>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="E37" s="1">
-        <f>(B37+C37)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.73668216768727846</v>
       </c>
       <c r="F37" s="1">
-        <f>-(C37)</f>
+        <f t="shared" si="5"/>
         <v>-134</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>63</v>
       </c>
@@ -3369,19 +3446,19 @@
         <v>33</v>
       </c>
       <c r="D38" s="1">
-        <f>B38-C38</f>
+        <f t="shared" si="3"/>
         <v>615</v>
       </c>
       <c r="E38" s="1">
-        <f>(B38+C38)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.5677517381094894</v>
       </c>
       <c r="F38" s="1">
-        <f>-(C38)</f>
+        <f t="shared" si="5"/>
         <v>-33</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>62</v>
       </c>
@@ -3392,19 +3469,19 @@
         <v>100</v>
       </c>
       <c r="D39" s="1">
-        <f>B39-C39</f>
+        <f t="shared" si="3"/>
         <v>441</v>
       </c>
       <c r="E39" s="1">
-        <f>(B39+C39)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.4756664671485795</v>
       </c>
       <c r="F39" s="1">
-        <f>-(C39)</f>
+        <f t="shared" si="5"/>
         <v>-100</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>61</v>
       </c>
@@ -3415,19 +3492,19 @@
         <v>68</v>
       </c>
       <c r="D40" s="1">
-        <f>B40-C40</f>
+        <f t="shared" si="3"/>
         <v>-31</v>
       </c>
       <c r="E40" s="1">
-        <f>(B40+C40)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.24172383627238822</v>
       </c>
       <c r="F40" s="1">
-        <f>-(C40)</f>
+        <f t="shared" si="5"/>
         <v>-68</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>60</v>
       </c>
@@ -3438,19 +3515,19 @@
         <v>163</v>
       </c>
       <c r="D41" s="1">
-        <f>B41-C41</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <f>(B41+C41)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.75049495833141489</v>
       </c>
       <c r="F41" s="1">
-        <f>-(C41)</f>
+        <f t="shared" si="5"/>
         <v>-163</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -3461,19 +3538,19 @@
         <v>133</v>
       </c>
       <c r="D42" s="1">
-        <f>B42-C42</f>
+        <f t="shared" si="3"/>
         <v>33</v>
       </c>
       <c r="E42" s="1">
-        <f>(B42+C42)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.68833740043280078</v>
       </c>
       <c r="F42" s="1">
-        <f>-(C42)</f>
+        <f t="shared" si="5"/>
         <v>-133</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
@@ -3484,19 +3561,19 @@
         <v>32</v>
       </c>
       <c r="D43" s="1">
-        <f>B43-C43</f>
+        <f t="shared" si="3"/>
         <v>519</v>
       </c>
       <c r="E43" s="1">
-        <f>(B43+C43)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.3421428242552604</v>
       </c>
       <c r="F43" s="1">
-        <f>-(C43)</f>
+        <f t="shared" si="5"/>
         <v>-32</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
@@ -3507,19 +3584,19 @@
         <v>211</v>
       </c>
       <c r="D44" s="1">
-        <f>B44-C44</f>
+        <f t="shared" si="3"/>
         <v>45</v>
       </c>
       <c r="E44" s="1">
-        <f>(B44+C44)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.075095538468622</v>
       </c>
       <c r="F44" s="1">
-        <f>-(C44)</f>
+        <f t="shared" si="5"/>
         <v>-211</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
@@ -3530,19 +3607,19 @@
         <v>438</v>
       </c>
       <c r="D45" s="1">
-        <f>B45-C45</f>
+        <f t="shared" si="3"/>
         <v>-151</v>
       </c>
       <c r="E45" s="1">
-        <f>(B45+C45)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.6690455361664902</v>
       </c>
       <c r="F45" s="1">
-        <f>-(C45)</f>
+        <f t="shared" si="5"/>
         <v>-438</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
@@ -3553,19 +3630,19 @@
         <v>122</v>
       </c>
       <c r="D46" s="1">
-        <f>B46-C46</f>
+        <f t="shared" si="3"/>
         <v>230</v>
       </c>
       <c r="E46" s="1">
-        <f>(B46+C46)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.0912104608867812</v>
       </c>
       <c r="F46" s="1">
-        <f>-(C46)</f>
+        <f t="shared" si="5"/>
         <v>-122</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -3576,19 +3653,19 @@
         <v>285</v>
       </c>
       <c r="D47" s="1">
-        <f>B47-C47</f>
+        <f t="shared" si="3"/>
         <v>-255</v>
       </c>
       <c r="E47" s="1">
-        <f>(B47+C47)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.72517150881716474</v>
       </c>
       <c r="F47" s="1">
-        <f>-(C47)</f>
+        <f t="shared" si="5"/>
         <v>-285</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>53</v>
       </c>
@@ -3599,19 +3676,19 @@
         <v>211</v>
       </c>
       <c r="D48" s="1">
-        <f>B48-C48</f>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="E48" s="1">
-        <f>(B48+C48)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.1602744141074635</v>
       </c>
       <c r="F48" s="1">
-        <f>-(C48)</f>
+        <f t="shared" si="5"/>
         <v>-211</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>52</v>
       </c>
@@ -3622,19 +3699,19 @@
         <v>15</v>
       </c>
       <c r="D49" s="1">
-        <f>B49-C49</f>
+        <f t="shared" si="3"/>
         <v>879</v>
       </c>
       <c r="E49" s="1">
-        <f>(B49+C49)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>2.0926377825866753</v>
       </c>
       <c r="F49" s="1">
-        <f>-(C49)</f>
+        <f t="shared" si="5"/>
         <v>-15</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -3645,19 +3722,19 @@
         <v>107</v>
       </c>
       <c r="D50" s="1">
-        <f>B50-C50</f>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="E50" s="1">
-        <f>(B50+C50)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.58013720705373173</v>
       </c>
       <c r="F50" s="1">
-        <f>-(C50)</f>
+        <f t="shared" si="5"/>
         <v>-107</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>50</v>
       </c>
@@ -3668,19 +3745,19 @@
         <v>497</v>
       </c>
       <c r="D51" s="1">
-        <f>B51-C51</f>
+        <f t="shared" si="3"/>
         <v>-446</v>
       </c>
       <c r="E51" s="1">
-        <f>(B51+C51)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.2615682121644642</v>
       </c>
       <c r="F51" s="1">
-        <f>-(C51)</f>
+        <f t="shared" si="5"/>
         <v>-497</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>49</v>
       </c>
@@ -3691,19 +3768,19 @@
         <v>60</v>
       </c>
       <c r="D52" s="1">
-        <f>B52-C52</f>
+        <f t="shared" si="3"/>
         <v>490</v>
       </c>
       <c r="E52" s="1">
-        <f>(B52+C52)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.4043003821538744</v>
       </c>
       <c r="F52" s="1">
-        <f>-(C52)</f>
+        <f t="shared" si="5"/>
         <v>-60</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>48</v>
       </c>
@@ -3714,19 +3791,19 @@
         <v>166</v>
       </c>
       <c r="D53" s="1">
-        <f>B53-C53</f>
+        <f t="shared" si="3"/>
         <v>300</v>
       </c>
       <c r="E53" s="1">
-        <f>(B53+C53)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.4549472811823749</v>
       </c>
       <c r="F53" s="1">
-        <f>-(C53)</f>
+        <f t="shared" si="5"/>
         <v>-166</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>47</v>
       </c>
@@ -3737,19 +3814,19 @@
         <v>421</v>
       </c>
       <c r="D54" s="1">
-        <f>B54-C54</f>
+        <f t="shared" si="3"/>
         <v>-366</v>
       </c>
       <c r="E54" s="1">
-        <f>(B54+C54)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.0958147244348266</v>
       </c>
       <c r="F54" s="1">
-        <f>-(C54)</f>
+        <f t="shared" si="5"/>
         <v>-421</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>46</v>
       </c>
@@ -3760,19 +3837,19 @@
         <v>268</v>
       </c>
       <c r="D55" s="1">
-        <f>B55-C55</f>
+        <f t="shared" si="3"/>
         <v>-108</v>
       </c>
       <c r="E55" s="1">
-        <f>(B55+C55)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.98531239928173486</v>
       </c>
       <c r="F55" s="1">
-        <f>-(C55)</f>
+        <f t="shared" si="5"/>
         <v>-268</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>45</v>
       </c>
@@ -3783,19 +3860,19 @@
         <v>85</v>
       </c>
       <c r="D56" s="1">
-        <f>B56-C56</f>
+        <f t="shared" si="3"/>
         <v>425</v>
       </c>
       <c r="E56" s="1">
-        <f>(B56+C56)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.3697684055435333</v>
       </c>
       <c r="F56" s="1">
-        <f>-(C56)</f>
+        <f t="shared" si="5"/>
         <v>-85</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>44</v>
       </c>
@@ -3806,19 +3883,19 @@
         <v>65</v>
       </c>
       <c r="D57" s="1">
-        <f>B57-C57</f>
+        <f t="shared" si="3"/>
         <v>249</v>
       </c>
       <c r="E57" s="1">
-        <f>(B57+C57)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.87250794235462037</v>
       </c>
       <c r="F57" s="1">
-        <f>-(C57)</f>
+        <f t="shared" si="5"/>
         <v>-65</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>43</v>
       </c>
@@ -3829,19 +3906,19 @@
         <v>61</v>
       </c>
       <c r="D58" s="1">
-        <f>B58-C58</f>
+        <f t="shared" si="3"/>
         <v>507</v>
       </c>
       <c r="E58" s="1">
-        <f>(B58+C58)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.4480408858603067</v>
       </c>
       <c r="F58" s="1">
-        <f>-(C58)</f>
+        <f t="shared" si="5"/>
         <v>-61</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>42</v>
       </c>
@@ -3852,19 +3929,19 @@
         <v>325</v>
       </c>
       <c r="D59" s="1">
-        <f>B59-C59</f>
+        <f t="shared" si="3"/>
         <v>-251</v>
       </c>
       <c r="E59" s="1">
-        <f>(B59+C59)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.91855057783507532</v>
       </c>
       <c r="F59" s="1">
-        <f>-(C59)</f>
+        <f t="shared" si="5"/>
         <v>-325</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>41</v>
       </c>
@@ -3875,19 +3952,19 @@
         <v>299</v>
       </c>
       <c r="D60" s="1">
-        <f>B60-C60</f>
+        <f t="shared" si="3"/>
         <v>-169</v>
       </c>
       <c r="E60" s="1">
-        <f>(B60+C60)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.98761453105575769</v>
       </c>
       <c r="F60" s="1">
-        <f>-(C60)</f>
+        <f t="shared" si="5"/>
         <v>-299</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>40</v>
       </c>
@@ -3898,19 +3975,19 @@
         <v>147</v>
       </c>
       <c r="D61" s="1">
-        <f>B61-C61</f>
+        <f t="shared" si="3"/>
         <v>253</v>
       </c>
       <c r="E61" s="1">
-        <f>(B61+C61)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.2592660803904416</v>
       </c>
       <c r="F61" s="1">
-        <f>-(C61)</f>
+        <f t="shared" si="5"/>
         <v>-147</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>39</v>
       </c>
@@ -3921,19 +3998,19 @@
         <v>471</v>
       </c>
       <c r="D62" s="1">
-        <f>B62-C62</f>
+        <f t="shared" si="3"/>
         <v>-450</v>
       </c>
       <c r="E62" s="1">
-        <f>(B62+C62)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.1326488328191906</v>
       </c>
       <c r="F62" s="1">
-        <f>-(C62)</f>
+        <f t="shared" si="5"/>
         <v>-471</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>38</v>
       </c>
@@ -3944,19 +4021,19 @@
         <v>292</v>
       </c>
       <c r="D63" s="1">
-        <f>B63-C63</f>
+        <f t="shared" si="3"/>
         <v>-88</v>
       </c>
       <c r="E63" s="1">
-        <f>(B63+C63)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>1.1418573599152815</v>
       </c>
       <c r="F63" s="1">
-        <f>-(C63)</f>
+        <f t="shared" si="5"/>
         <v>-292</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>37</v>
       </c>
@@ -3967,19 +4044,19 @@
         <v>116</v>
       </c>
       <c r="D64" s="1">
-        <f>B64-C64</f>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="E64" s="1">
-        <f>(B64+C64)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.66071181914452781</v>
       </c>
       <c r="F64" s="1">
-        <f>-(C64)</f>
+        <f t="shared" si="5"/>
         <v>-116</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>36</v>
       </c>
@@ -3990,19 +4067,19 @@
         <v>128</v>
       </c>
       <c r="D65" s="1">
-        <f>B65-C65</f>
+        <f t="shared" si="3"/>
         <v>91</v>
       </c>
       <c r="E65" s="1">
-        <f>(B65+C65)/(434.38)</f>
+        <f t="shared" si="4"/>
         <v>0.79883972558589256</v>
       </c>
       <c r="F65" s="1">
-        <f>-(C65)</f>
+        <f t="shared" si="5"/>
         <v>-128</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>35</v>
       </c>
@@ -4013,19 +4090,19 @@
         <v>415</v>
       </c>
       <c r="D66" s="1">
-        <f>B66-C66</f>
+        <f t="shared" ref="D66:D87" si="6">B66-C66</f>
         <v>-377</v>
       </c>
       <c r="E66" s="1">
-        <f>(B66+C66)/(434.38)</f>
+        <f t="shared" ref="E66:E87" si="7">(B66+C66)/(434.38)</f>
         <v>1.0428656936323035</v>
       </c>
       <c r="F66" s="1">
-        <f>-(C66)</f>
+        <f t="shared" ref="F66:F87" si="8">-(C66)</f>
         <v>-415</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>34</v>
       </c>
@@ -4036,19 +4113,19 @@
         <v>207</v>
       </c>
       <c r="D67" s="1">
-        <f>B67-C67</f>
+        <f t="shared" si="6"/>
         <v>-19</v>
       </c>
       <c r="E67" s="1">
-        <f>(B67+C67)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>0.90934205073898433</v>
       </c>
       <c r="F67" s="1">
-        <f>-(C67)</f>
+        <f t="shared" si="8"/>
         <v>-207</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>33</v>
       </c>
@@ -4059,19 +4136,19 @@
         <v>225</v>
       </c>
       <c r="D68" s="1">
-        <f>B68-C68</f>
+        <f t="shared" si="6"/>
         <v>47</v>
       </c>
       <c r="E68" s="1">
-        <f>(B68+C68)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.1441594916893043</v>
       </c>
       <c r="F68" s="1">
-        <f>-(C68)</f>
+        <f t="shared" si="8"/>
         <v>-225</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>32</v>
       </c>
@@ -4082,19 +4159,19 @@
         <v>586</v>
       </c>
       <c r="D69" s="1">
-        <f>B69-C69</f>
+        <f t="shared" si="6"/>
         <v>-543</v>
       </c>
       <c r="E69" s="1">
-        <f>(B69+C69)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.4480408858603067</v>
       </c>
       <c r="F69" s="1">
-        <f>-(C69)</f>
+        <f t="shared" si="8"/>
         <v>-586</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>31</v>
       </c>
@@ -4105,19 +4182,19 @@
         <v>82</v>
       </c>
       <c r="D70" s="1">
-        <f>B70-C70</f>
+        <f t="shared" si="6"/>
         <v>504</v>
       </c>
       <c r="E70" s="1">
-        <f>(B70+C70)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.5378240250471937</v>
       </c>
       <c r="F70" s="1">
-        <f>-(C70)</f>
+        <f t="shared" si="8"/>
         <v>-82</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>30</v>
       </c>
@@ -4128,19 +4205,19 @@
         <v>607</v>
       </c>
       <c r="D71" s="1">
-        <f>B71-C71</f>
+        <f t="shared" si="6"/>
         <v>-481</v>
       </c>
       <c r="E71" s="1">
-        <f>(B71+C71)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.6874625903586722</v>
       </c>
       <c r="F71" s="1">
-        <f>-(C71)</f>
+        <f t="shared" si="8"/>
         <v>-607</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>29</v>
       </c>
@@ -4151,19 +4228,19 @@
         <v>285</v>
       </c>
       <c r="D72" s="1">
-        <f>B72-C72</f>
+        <f t="shared" si="6"/>
         <v>-153</v>
       </c>
       <c r="E72" s="1">
-        <f>(B72+C72)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>0.95998894976748472</v>
       </c>
       <c r="F72" s="1">
-        <f>-(C72)</f>
+        <f t="shared" si="8"/>
         <v>-285</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>28</v>
       </c>
@@ -4174,19 +4251,19 @@
         <v>43</v>
       </c>
       <c r="D73" s="1">
-        <f>B73-C73</f>
+        <f t="shared" si="6"/>
         <v>599</v>
       </c>
       <c r="E73" s="1">
-        <f>(B73+C73)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.5769602652055803</v>
       </c>
       <c r="F73" s="1">
-        <f>-(C73)</f>
+        <f t="shared" si="8"/>
         <v>-43</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>27</v>
       </c>
@@ -4197,19 +4274,19 @@
         <v>33</v>
       </c>
       <c r="D74" s="1">
-        <f>B74-C74</f>
+        <f t="shared" si="6"/>
         <v>460</v>
       </c>
       <c r="E74" s="1">
-        <f>(B74+C74)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.210921313135964</v>
       </c>
       <c r="F74" s="1">
-        <f>-(C74)</f>
+        <f t="shared" si="8"/>
         <v>-33</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>26</v>
       </c>
@@ -4220,19 +4297,19 @@
         <v>621</v>
       </c>
       <c r="D75" s="1">
-        <f>B75-C75</f>
+        <f t="shared" si="6"/>
         <v>-592</v>
       </c>
       <c r="E75" s="1">
-        <f>(B75+C75)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.4963856531147843</v>
       </c>
       <c r="F75" s="1">
-        <f>-(C75)</f>
+        <f t="shared" si="8"/>
         <v>-621</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>25</v>
       </c>
@@ -4243,19 +4320,19 @@
         <v>327</v>
       </c>
       <c r="D76" s="1">
-        <f>B76-C76</f>
+        <f t="shared" si="6"/>
         <v>130</v>
       </c>
       <c r="E76" s="1">
-        <f>(B76+C76)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.8048713108338321</v>
       </c>
       <c r="F76" s="1">
-        <f>-(C76)</f>
+        <f t="shared" si="8"/>
         <v>-327</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>24</v>
       </c>
@@ -4266,19 +4343,19 @@
         <v>144</v>
       </c>
       <c r="D77" s="1">
-        <f>B77-C77</f>
+        <f t="shared" si="6"/>
         <v>435</v>
       </c>
       <c r="E77" s="1">
-        <f>(B77+C77)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.6644412726184448</v>
       </c>
       <c r="F77" s="1">
-        <f>-(C77)</f>
+        <f t="shared" si="8"/>
         <v>-144</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>23</v>
       </c>
@@ -4289,19 +4366,19 @@
         <v>277</v>
       </c>
       <c r="D78" s="1">
-        <f>B78-C78</f>
+        <f t="shared" si="6"/>
         <v>-162</v>
       </c>
       <c r="E78" s="1">
-        <f>(B78+C78)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>0.90243565541691606</v>
       </c>
       <c r="F78" s="1">
-        <f>-(C78)</f>
+        <f t="shared" si="8"/>
         <v>-277</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>22</v>
       </c>
@@ -4312,19 +4389,19 @@
         <v>579</v>
       </c>
       <c r="D79" s="1">
-        <f>B79-C79</f>
+        <f t="shared" si="6"/>
         <v>-565</v>
       </c>
       <c r="E79" s="1">
-        <f>(B79+C79)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.3651641419954879</v>
       </c>
       <c r="F79" s="1">
-        <f>-(C79)</f>
+        <f t="shared" si="8"/>
         <v>-579</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>21</v>
       </c>
@@ -4335,19 +4412,19 @@
         <v>281</v>
       </c>
       <c r="D80" s="1">
-        <f>B80-C80</f>
+        <f t="shared" si="6"/>
         <v>-166</v>
       </c>
       <c r="E80" s="1">
-        <f>(B80+C80)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>0.91164418251300705</v>
       </c>
       <c r="F80" s="1">
-        <f>-(C80)</f>
+        <f t="shared" si="8"/>
         <v>-281</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>20</v>
       </c>
@@ -4358,19 +4435,19 @@
         <v>585</v>
       </c>
       <c r="D81" s="1">
-        <f>B81-C81</f>
+        <f t="shared" si="6"/>
         <v>-538</v>
       </c>
       <c r="E81" s="1">
-        <f>(B81+C81)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.4549472811823749</v>
       </c>
       <c r="F81" s="1">
-        <f>-(C81)</f>
+        <f t="shared" si="8"/>
         <v>-585</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>19</v>
       </c>
@@ -4381,19 +4458,19 @@
         <v>219</v>
       </c>
       <c r="D82" s="1">
-        <f>B82-C82</f>
+        <f t="shared" si="6"/>
         <v>81</v>
       </c>
       <c r="E82" s="1">
-        <f>(B82+C82)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.1948063907178046</v>
       </c>
       <c r="F82" s="1">
-        <f>-(C82)</f>
+        <f t="shared" si="8"/>
         <v>-219</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>18</v>
       </c>
@@ -4404,19 +4481,19 @@
         <v>99</v>
       </c>
       <c r="D83" s="1">
-        <f>B83-C83</f>
+        <f t="shared" si="6"/>
         <v>-68</v>
       </c>
       <c r="E83" s="1">
-        <f>(B83+C83)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>0.29927713062295686</v>
       </c>
       <c r="F83" s="1">
-        <f>-(C83)</f>
+        <f t="shared" si="8"/>
         <v>-99</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>17</v>
       </c>
@@ -4427,19 +4504,19 @@
         <v>252</v>
       </c>
       <c r="D84" s="1">
-        <f>B84-C84</f>
+        <f t="shared" si="6"/>
         <v>-218</v>
       </c>
       <c r="E84" s="1">
-        <f>(B84+C84)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>0.65840968737050509</v>
       </c>
       <c r="F84" s="1">
-        <f>-(C84)</f>
+        <f t="shared" si="8"/>
         <v>-252</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>16</v>
       </c>
@@ -4450,19 +4527,19 @@
         <v>13</v>
       </c>
       <c r="D85" s="1">
-        <f>B85-C85</f>
+        <f t="shared" si="6"/>
         <v>815</v>
       </c>
       <c r="E85" s="1">
-        <f>(B85+C85)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.9360928219531286</v>
       </c>
       <c r="F85" s="1">
-        <f>-(C85)</f>
+        <f t="shared" si="8"/>
         <v>-13</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>8</v>
       </c>
@@ -4473,19 +4550,19 @@
         <v>663</v>
       </c>
       <c r="D86" s="1">
-        <f>B86-C86</f>
+        <f t="shared" si="6"/>
         <v>-543</v>
       </c>
       <c r="E86" s="1">
-        <f>(B86+C86)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.8025691790598095</v>
       </c>
       <c r="F86" s="1">
-        <f>-(C86)</f>
+        <f t="shared" si="8"/>
         <v>-663</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
@@ -4496,19 +4573,19 @@
         <v>34</v>
       </c>
       <c r="D87" s="1">
-        <f>B87-C87</f>
+        <f t="shared" si="6"/>
         <v>536</v>
       </c>
       <c r="E87" s="1">
-        <f>(B87+C87)/(434.38)</f>
+        <f t="shared" si="7"/>
         <v>1.3904875915097381</v>
       </c>
       <c r="F87" s="1">
-        <f>-(C87)</f>
+        <f t="shared" si="8"/>
         <v>-34</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
         <v>26204</v>
       </c>
@@ -4517,17 +4594,16 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <sortState ref="A2:F88">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F88">
     <sortCondition descending="1" ref="A3:A88"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;LDATA: Candy Hierarchy (Oct 29th, 11:48am | 11:51am) </oddHeader>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="1" OnePage="0" WScale="0"/>

</xml_diff>